<commit_message>
New changes as of 04/15
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC01_CDS_phs001287.xlsx
+++ b/InputFiles/CDS/TC01_CDS_phs001287.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0925\Commons_Automation\InputFiles\CDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0305\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AD2E26-4908-4774-A9E8-4B3C68C4B948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C248ACD6-4064-496D-9B11-89D50ED7C40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,8 +129,7 @@
     f1.file_type,
     gi.library_strategy
 ORDER BY 
-    f1.file_name ASC
-LIMIT 100;</t>
+    f1.file_name ASC;</t>
   </si>
   <si>
     <t>SELECT
@@ -156,7 +155,7 @@
     s.phs_accession = 'phs001287'
 ORDER BY 
     smp.sample_id ASC
-LIMIT 100;</t>
+;</t>
   </si>
   <si>
     <t>WITH Distinct_Samples AS (
@@ -220,7 +219,7 @@
     study_name,
     phs_accession,
     gender
-LIMIT 100;</t>
+;</t>
   </si>
 </sst>
 </file>
@@ -613,7 +612,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>